<commit_message>
seem to have changed something on the wrapping
</commit_message>
<xml_diff>
--- a/OtherStuff/JSWrapping.xlsx
+++ b/OtherStuff/JSWrapping.xlsx
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>wrapObject</t>
-  </si>
-  <si>
-    <t>JSObjToClassPtr</t>
   </si>
   <si>
     <t>isKJS</t>
@@ -360,6 +357,9 @@
   </si>
   <si>
     <t>uncommon</t>
+  </si>
+  <si>
+    <t>unwrappable</t>
   </si>
 </sst>
 </file>
@@ -739,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A9:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -755,7 +755,7 @@
   <sheetData>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>0</v>
@@ -767,126 +767,126 @@
         <v>4</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -900,7 +900,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -912,438 +912,438 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H23" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="4" customFormat="1"/>
     <row r="25" spans="1:9" s="4" customFormat="1">
       <c r="A25" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I33" s="4"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H37" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I37" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1358,7 +1358,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1370,158 +1370,158 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1536,7 +1536,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1548,164 +1548,164 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G48" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G51" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H51" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="H51" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -1720,7 +1720,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -1732,290 +1732,290 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C63" t="s">
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H63" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C64" t="s">
         <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H64" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C65" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D65" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" t="s">
         <v>11</v>
       </c>
-      <c r="E65" t="s">
-        <v>12</v>
-      </c>
       <c r="F65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H65" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="C66" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D66" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H66" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="H67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="B68" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D68" t="s">
+        <v>22</v>
+      </c>
+      <c r="H68" t="s">
         <v>23</v>
-      </c>
-      <c r="H68" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="F69" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H69" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="H70" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="H71" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>